<commit_message>
- bc congno chitiet: add {NoThucTe}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_BaoCaoCongNoChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_BaoCaoCongNoChiTiet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t>BÁO CÁO CHI TIẾT CÔNG NỢ KHÁCH HÀNG</t>
+  </si>
+  <si>
+    <t>Nợ thực tế</t>
   </si>
 </sst>
 </file>
@@ -63,7 +66,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-101042A]d/m/yyyy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-101042A]d/m/yyyy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -170,49 +173,49 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -520,65 +523,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="12" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" style="21" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" style="12" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="14" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" style="14" customWidth="1"/>
-    <col min="8" max="9" width="31.28515625" style="12" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" style="12" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="23.7109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="15" customWidth="1"/>
+    <col min="6" max="7" width="22.7109375" style="12" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="12" customWidth="1"/>
+    <col min="9" max="10" width="31.28515625" style="10" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="10" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -590,333 +595,364 @@
       <c r="G4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="J4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="K4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="15"/>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="13"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="15"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="13"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="15"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="13"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="15"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="13"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="H8" s="5"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="15"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="13"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="15"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="13"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="15"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="15"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="13"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="15"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="13"/>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="15"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="13"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="15"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="15"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="13"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="15"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="13"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="15"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="13"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="15"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="13"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="19"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="15"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="13"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
-      <c r="B21" s="19"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="15"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="13"/>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
-      <c r="B22" s="19"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="15"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="13"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="15"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="13"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="15"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="13"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="B25" s="19"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="15"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="13"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="15"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="13"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="15"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="13"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-    </row>
-    <row r="28" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="19"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="15"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="13"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="10"/>
-    </row>
-    <row r="29" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="H28" s="5"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="16">
-        <f>SUM(E$6:E28)</f>
+      <c r="B29" s="18"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="14">
+        <f>SUM(E$5:E28)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="16">
-        <f>SUM(F$6:F28)</f>
+      <c r="F29" s="14">
+        <f>SUM(F$5:F28)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="16">
-        <f>SUM(G$6:G28)</f>
+      <c r="G29" s="14">
+        <f>SUM(G$5:G28)</f>
         <v>0</v>
       </c>
-      <c r="H29" s="13"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
+      <c r="H29" s="14">
+        <f>SUM(H$5:H28)</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
- BC congno chitiet: add column {NVPhuTrach}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_BaoCaoCongNoChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_BaoCaoCongNoChiTiet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Nợ thực tế</t>
+  </si>
+  <si>
+    <t>NV phụ trách</t>
   </si>
 </sst>
 </file>
@@ -523,11 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,16 +538,17 @@
     <col min="1" max="1" width="23.7109375" style="10" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="19" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" style="15" customWidth="1"/>
-    <col min="6" max="7" width="22.7109375" style="12" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="12" customWidth="1"/>
-    <col min="9" max="10" width="31.28515625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" style="10" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="40" style="10" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="10" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="15" customWidth="1"/>
+    <col min="7" max="8" width="22.7109375" style="12" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" style="12" customWidth="1"/>
+    <col min="10" max="11" width="31.28515625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" style="10" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
@@ -558,9 +562,10 @@
       <c r="I1" s="20"/>
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
-      <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="20"/>
+      <c r="M1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -572,8 +577,9 @@
       <c r="I2" s="21"/>
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
-    </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L2" s="21"/>
+    </row>
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -586,353 +592,377 @@
       <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="L4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="17"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="5"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
-      <c r="I5" s="8"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="17"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="5"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
-      <c r="I6" s="8"/>
+      <c r="I6" s="5"/>
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="17"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="13"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-      <c r="I7" s="8"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="17"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="13"/>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-      <c r="I8" s="8"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="17"/>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="8"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="17"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
-      <c r="I10" s="8"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="17"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
-      <c r="I11" s="8"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="17"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
-      <c r="I12" s="8"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="17"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-      <c r="I13" s="8"/>
+      <c r="I13" s="5"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="17"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="8"/>
+      <c r="I14" s="5"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="17"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="5"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="8"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L15" s="8"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="17"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="5"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="8"/>
+      <c r="I16" s="5"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="8"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="17"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="8"/>
+      <c r="I17" s="5"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="8"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="17"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="13"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
-      <c r="I18" s="8"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="17"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="5"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="8"/>
+      <c r="I19" s="5"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="8"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="17"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="5"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-      <c r="I20" s="8"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="8"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="17"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="5"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="13"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
-      <c r="I21" s="8"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="8"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="17"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="5"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="5"/>
       <c r="H22" s="5"/>
-      <c r="I22" s="8"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="17"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="5"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="13"/>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
-      <c r="I23" s="8"/>
+      <c r="I23" s="5"/>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="8"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="17"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="5"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="13"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
-      <c r="I24" s="8"/>
+      <c r="I24" s="5"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="17"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="5"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="13"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
-      <c r="I25" s="8"/>
+      <c r="I25" s="5"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="8"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="17"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="5"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="13"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
-      <c r="I26" s="8"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="8"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="17"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="5"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="13"/>
       <c r="G27" s="5"/>
       <c r="H27" s="5"/>
-      <c r="I27" s="8"/>
+      <c r="I27" s="5"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
-    </row>
-    <row r="28" spans="1:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="L27" s="8"/>
+    </row>
+    <row r="28" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="17"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="5"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="13"/>
       <c r="G28" s="5"/>
       <c r="H28" s="5"/>
-      <c r="I28" s="8"/>
+      <c r="I28" s="5"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L28" s="8"/>
+    </row>
+    <row r="29" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="18"/>
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
-      <c r="E29" s="14">
-        <f>SUM(E$5:E28)</f>
-        <v>0</v>
-      </c>
+      <c r="E29" s="11"/>
       <c r="F29" s="14">
         <f>SUM(F$5:F28)</f>
         <v>0</v>
@@ -945,14 +975,18 @@
         <f>SUM(H$5:H28)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="11"/>
+      <c r="I29" s="14">
+        <f>SUM(I$5:I28)</f>
+        <v>0</v>
+      </c>
       <c r="J29" s="11"/>
       <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:L2"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
BC taichinh - congno chitiet: add column {BuTruTraHang, MaHoaDonTra}
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_BaoCaoCongNoChiTiet.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoTaiChinh/Teamplate_BaoCaoCongNoChiTiet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>NV phụ trách</t>
+  </si>
+  <si>
+    <t>Bù trừ trả hàng</t>
+  </si>
+  <si>
+    <t>Mã hóa đơn trả</t>
+  </si>
+  <si>
+    <t>Giá trị sau trả</t>
   </si>
 </sst>
 </file>
@@ -526,11 +535,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,15 +549,15 @@
     <col min="3" max="3" width="21.28515625" style="10" customWidth="1"/>
     <col min="4" max="4" width="40" style="10" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" style="15" customWidth="1"/>
-    <col min="7" max="8" width="22.7109375" style="12" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" style="12" customWidth="1"/>
-    <col min="10" max="11" width="31.28515625" style="10" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="10" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="6" max="9" width="21.85546875" style="15" customWidth="1"/>
+    <col min="10" max="11" width="22.7109375" style="12" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="12" customWidth="1"/>
+    <col min="13" max="14" width="31.28515625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="22.7109375" style="10" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>12</v>
       </c>
@@ -563,9 +572,12 @@
       <c r="J1" s="20"/>
       <c r="K1" s="20"/>
       <c r="L1" s="20"/>
-      <c r="M1" s="2"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -578,8 +590,11 @@
       <c r="J2" s="21"/>
       <c r="K2" s="21"/>
       <c r="L2" s="21"/>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+    </row>
+    <row r="4" spans="1:16" s="3" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
@@ -599,81 +614,102 @@
         <v>6</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="M4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="N4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="O4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="17"/>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="13"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="17"/>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="13"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="17"/>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="13"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="17"/>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="13"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
@@ -682,280 +718,340 @@
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="17"/>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="17"/>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="17"/>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="17"/>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="17"/>
       <c r="C14" s="8"/>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="13"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="17"/>
       <c r="C15" s="8"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="17"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="13"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="17"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="8"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="17"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="13"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="17"/>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="13"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="8"/>
       <c r="B20" s="17"/>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="13"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="17"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="17"/>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="13"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="17"/>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
       <c r="E23" s="8"/>
       <c r="F23" s="13"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="8"/>
       <c r="B24" s="17"/>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="8"/>
       <c r="F24" s="13"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="17"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="8"/>
       <c r="F25" s="13"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="8"/>
+      <c r="N25" s="8"/>
+      <c r="O25" s="8"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="17"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="13"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="8"/>
+      <c r="N26" s="8"/>
+      <c r="O26" s="8"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="8"/>
       <c r="B27" s="17"/>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
       <c r="E27" s="8"/>
       <c r="F27" s="13"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-    </row>
-    <row r="28" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
+    </row>
+    <row r="28" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="17"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="13"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-    </row>
-    <row r="29" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="8"/>
+      <c r="N28" s="8"/>
+      <c r="O28" s="8"/>
+    </row>
+    <row r="29" spans="1:15" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>1</v>
       </c>
@@ -971,22 +1067,31 @@
         <f>SUM(G$5:G28)</f>
         <v>0</v>
       </c>
-      <c r="H29" s="14">
-        <f>SUM(H$5:H28)</f>
-        <v>0</v>
-      </c>
+      <c r="H29" s="14"/>
       <c r="I29" s="14">
         <f>SUM(I$5:I28)</f>
         <v>0</v>
       </c>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
+      <c r="J29" s="14">
+        <f>SUM(J$5:J28)</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="14">
+        <f>SUM(K$5:K28)</f>
+        <v>0</v>
+      </c>
+      <c r="L29" s="14">
+        <f>SUM(L$5:L28)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="A2:O2"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>